<commit_message>
Update all of the schedule .xlsx files using schoolAndPlanURLs[0]
</commit_message>
<xml_diff>
--- a/py_version/schedules/schedule-lists_owners-grouped.xlsx
+++ b/py_version/schedules/schedule-lists_owners-grouped.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="classrooms" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="subjects" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="teachers" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="classrooms" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="subjects" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="teachers" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1101,7 +1101,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E143"/>
+  <dimension ref="A1:E79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1112,7 +1112,7 @@
     <col width="11" customWidth="1" min="1" max="1"/>
     <col width="13" customWidth="1" min="2" max="2"/>
     <col width="20" customWidth="1" min="3" max="3"/>
-    <col width="17" customWidth="1" min="4" max="4"/>
+    <col width="13" customWidth="1" min="4" max="4"/>
     <col width="11" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
@@ -1178,7 +1178,7 @@
       </c>
       <c r="D3" s="6" t="inlineStr">
         <is>
-          <t>ang-ek</t>
+          <t>ang-fry</t>
         </is>
       </c>
       <c r="E3" s="6" t="n">
@@ -1195,7 +1195,7 @@
       </c>
       <c r="D4" s="6" t="inlineStr">
         <is>
-          <t>ang-fry</t>
+          <t>ang-gas</t>
         </is>
       </c>
       <c r="E4" s="6" t="n">
@@ -1212,7 +1212,7 @@
       </c>
       <c r="D5" s="6" t="inlineStr">
         <is>
-          <t>ang-fry-fry</t>
+          <t>ang-hot</t>
         </is>
       </c>
       <c r="E5" s="6" t="n">
@@ -1229,7 +1229,7 @@
       </c>
       <c r="D6" s="6" t="inlineStr">
         <is>
-          <t>ang-gas</t>
+          <t>ang-log</t>
         </is>
       </c>
       <c r="E6" s="6" t="n">
@@ -1246,7 +1246,7 @@
       </c>
       <c r="D7" s="6" t="inlineStr">
         <is>
-          <t>ang-gas-gas</t>
+          <t>ang-ra</t>
         </is>
       </c>
       <c r="E7" s="6" t="n">
@@ -1254,8 +1254,8 @@
       </c>
     </row>
     <row r="8" ht="14.3" customHeight="1">
-      <c r="A8" s="8" t="n"/>
-      <c r="B8" s="8" t="n"/>
+      <c r="A8" s="9" t="n"/>
+      <c r="B8" s="9" t="n"/>
       <c r="C8" s="5" t="inlineStr">
         <is>
           <t>7.</t>
@@ -1263,7 +1263,7 @@
       </c>
       <c r="D8" s="6" t="inlineStr">
         <is>
-          <t>ang-hot</t>
+          <t>ang.r</t>
         </is>
       </c>
       <c r="E8" s="6" t="n">
@@ -1271,33 +1271,49 @@
       </c>
     </row>
     <row r="9" ht="14.3" customHeight="1">
-      <c r="A9" s="8" t="n"/>
-      <c r="B9" s="8" t="n"/>
-      <c r="C9" s="5" t="inlineStr">
-        <is>
-          <t>8.</t>
-        </is>
-      </c>
-      <c r="D9" s="6" t="inlineStr">
-        <is>
-          <t>ang-hot-hot</t>
-        </is>
-      </c>
-      <c r="E9" s="6" t="n">
+      <c r="A9" s="4" t="inlineStr">
+        <is>
+          <t>2.</t>
+        </is>
+      </c>
+      <c r="B9" s="4" t="inlineStr">
+        <is>
+          <t>b.h.p</t>
+        </is>
+      </c>
+      <c r="C9" s="4" t="inlineStr">
+        <is>
+          <t>1.</t>
+        </is>
+      </c>
+      <c r="D9" s="7" t="inlineStr">
+        <is>
+          <t>b.h.p</t>
+        </is>
+      </c>
+      <c r="E9" s="7" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="10" ht="14.3" customHeight="1">
-      <c r="A10" s="8" t="n"/>
-      <c r="B10" s="8" t="n"/>
+      <c r="A10" s="5" t="inlineStr">
+        <is>
+          <t>3.</t>
+        </is>
+      </c>
+      <c r="B10" s="5" t="inlineStr">
+        <is>
+          <t>b.i.z</t>
+        </is>
+      </c>
       <c r="C10" s="5" t="inlineStr">
         <is>
-          <t>9.</t>
+          <t>1.</t>
         </is>
       </c>
       <c r="D10" s="6" t="inlineStr">
         <is>
-          <t>ang-j1</t>
+          <t>b.i.z</t>
         </is>
       </c>
       <c r="E10" s="6" t="n">
@@ -1305,50 +1321,66 @@
       </c>
     </row>
     <row r="11" ht="14.3" customHeight="1">
-      <c r="A11" s="8" t="n"/>
-      <c r="B11" s="8" t="n"/>
-      <c r="C11" s="5" t="inlineStr">
-        <is>
-          <t>10.</t>
-        </is>
-      </c>
-      <c r="D11" s="6" t="inlineStr">
-        <is>
-          <t>ang-j2</t>
-        </is>
-      </c>
-      <c r="E11" s="6" t="n">
+      <c r="A11" s="4" t="inlineStr">
+        <is>
+          <t>4.</t>
+        </is>
+      </c>
+      <c r="B11" s="4" t="inlineStr">
+        <is>
+          <t>biol</t>
+        </is>
+      </c>
+      <c r="C11" s="4" t="inlineStr">
+        <is>
+          <t>1.</t>
+        </is>
+      </c>
+      <c r="D11" s="7" t="inlineStr">
+        <is>
+          <t>biol.r</t>
+        </is>
+      </c>
+      <c r="E11" s="7" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="12" ht="14.3" customHeight="1">
-      <c r="A12" s="8" t="n"/>
-      <c r="B12" s="8" t="n"/>
-      <c r="C12" s="5" t="inlineStr">
-        <is>
-          <t>11.</t>
-        </is>
-      </c>
-      <c r="D12" s="6" t="inlineStr">
-        <is>
-          <t>ang-log</t>
-        </is>
-      </c>
-      <c r="E12" s="6" t="n">
+      <c r="A12" s="9" t="n"/>
+      <c r="B12" s="9" t="n"/>
+      <c r="C12" s="4" t="inlineStr">
+        <is>
+          <t>2.</t>
+        </is>
+      </c>
+      <c r="D12" s="7" t="inlineStr">
+        <is>
+          <t>biologia</t>
+        </is>
+      </c>
+      <c r="E12" s="7" t="n">
         <v>11</v>
       </c>
     </row>
     <row r="13" ht="14.3" customHeight="1">
-      <c r="A13" s="8" t="n"/>
-      <c r="B13" s="8" t="n"/>
+      <c r="A13" s="5" t="inlineStr">
+        <is>
+          <t>5.</t>
+        </is>
+      </c>
+      <c r="B13" s="5" t="inlineStr">
+        <is>
+          <t>chemia</t>
+        </is>
+      </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>12.</t>
+          <t>1.</t>
         </is>
       </c>
       <c r="D13" s="6" t="inlineStr">
         <is>
-          <t>ang-log-log</t>
+          <t>chemia</t>
         </is>
       </c>
       <c r="E13" s="6" t="n">
@@ -1356,33 +1388,49 @@
       </c>
     </row>
     <row r="14" ht="14.3" customHeight="1">
-      <c r="A14" s="8" t="n"/>
-      <c r="B14" s="8" t="n"/>
-      <c r="C14" s="5" t="inlineStr">
-        <is>
-          <t>13.</t>
-        </is>
-      </c>
-      <c r="D14" s="6" t="inlineStr">
-        <is>
-          <t>ang-ra</t>
-        </is>
-      </c>
-      <c r="E14" s="6" t="n">
+      <c r="A14" s="4" t="inlineStr">
+        <is>
+          <t>6.</t>
+        </is>
+      </c>
+      <c r="B14" s="4" t="inlineStr">
+        <is>
+          <t>dok.r.pr.tr</t>
+        </is>
+      </c>
+      <c r="C14" s="4" t="inlineStr">
+        <is>
+          <t>1.</t>
+        </is>
+      </c>
+      <c r="D14" s="7" t="inlineStr">
+        <is>
+          <t>dok.r.pr.tr</t>
+        </is>
+      </c>
+      <c r="E14" s="7" t="n">
         <v>13</v>
       </c>
     </row>
     <row r="15" ht="14.3" customHeight="1">
-      <c r="A15" s="8" t="n"/>
-      <c r="B15" s="8" t="n"/>
+      <c r="A15" s="5" t="inlineStr">
+        <is>
+          <t>7.</t>
+        </is>
+      </c>
+      <c r="B15" s="5" t="inlineStr">
+        <is>
+          <t>dok.zd.gos</t>
+        </is>
+      </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>14.</t>
+          <t>1.</t>
         </is>
       </c>
       <c r="D15" s="6" t="inlineStr">
         <is>
-          <t>ang-ra-ra</t>
+          <t>dok.zd.gos</t>
         </is>
       </c>
       <c r="E15" s="6" t="n">
@@ -1390,58 +1438,74 @@
       </c>
     </row>
     <row r="16" ht="14.3" customHeight="1">
-      <c r="A16" s="9" t="n"/>
-      <c r="B16" s="9" t="n"/>
-      <c r="C16" s="5" t="inlineStr">
-        <is>
-          <t>15.</t>
-        </is>
-      </c>
-      <c r="D16" s="6" t="inlineStr">
-        <is>
-          <t>ang.r</t>
-        </is>
-      </c>
-      <c r="E16" s="6" t="n">
+      <c r="A16" s="4" t="inlineStr">
+        <is>
+          <t>8.</t>
+        </is>
+      </c>
+      <c r="B16" s="4" t="inlineStr">
+        <is>
+          <t>dz.w.rec</t>
+        </is>
+      </c>
+      <c r="C16" s="4" t="inlineStr">
+        <is>
+          <t>1.</t>
+        </is>
+      </c>
+      <c r="D16" s="7" t="inlineStr">
+        <is>
+          <t>dz.w.rec</t>
+        </is>
+      </c>
+      <c r="E16" s="7" t="n">
         <v>15</v>
       </c>
     </row>
     <row r="17" ht="14.3" customHeight="1">
-      <c r="A17" s="4" t="inlineStr">
-        <is>
-          <t>2.</t>
-        </is>
-      </c>
-      <c r="B17" s="4" t="inlineStr">
-        <is>
-          <t>b.h.p</t>
-        </is>
-      </c>
-      <c r="C17" s="4" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D17" s="7" t="inlineStr">
-        <is>
-          <t>b.h.p</t>
-        </is>
-      </c>
-      <c r="E17" s="7" t="n">
+      <c r="A17" s="5" t="inlineStr">
+        <is>
+          <t>9.</t>
+        </is>
+      </c>
+      <c r="B17" s="5" t="inlineStr">
+        <is>
+          <t>e.d.b</t>
+        </is>
+      </c>
+      <c r="C17" s="5" t="inlineStr">
+        <is>
+          <t>1.</t>
+        </is>
+      </c>
+      <c r="D17" s="6" t="inlineStr">
+        <is>
+          <t>e.d.b</t>
+        </is>
+      </c>
+      <c r="E17" s="6" t="n">
         <v>16</v>
       </c>
     </row>
     <row r="18" ht="14.3" customHeight="1">
-      <c r="A18" s="8" t="n"/>
-      <c r="B18" s="8" t="n"/>
+      <c r="A18" s="4" t="inlineStr">
+        <is>
+          <t>10.</t>
+        </is>
+      </c>
+      <c r="B18" s="4" t="inlineStr">
+        <is>
+          <t>f.p.gos</t>
+        </is>
+      </c>
       <c r="C18" s="4" t="inlineStr">
         <is>
-          <t>2.</t>
+          <t>1.</t>
         </is>
       </c>
       <c r="D18" s="7" t="inlineStr">
         <is>
-          <t>b.h.p-ek</t>
+          <t>f.p.gos</t>
         </is>
       </c>
       <c r="E18" s="7" t="n">
@@ -1449,33 +1513,49 @@
       </c>
     </row>
     <row r="19" ht="14.3" customHeight="1">
-      <c r="A19" s="8" t="n"/>
-      <c r="B19" s="8" t="n"/>
-      <c r="C19" s="4" t="inlineStr">
-        <is>
-          <t>3.</t>
-        </is>
-      </c>
-      <c r="D19" s="7" t="inlineStr">
-        <is>
-          <t>b.h.p-gas</t>
-        </is>
-      </c>
-      <c r="E19" s="7" t="n">
+      <c r="A19" s="5" t="inlineStr">
+        <is>
+          <t>11.</t>
+        </is>
+      </c>
+      <c r="B19" s="5" t="inlineStr">
+        <is>
+          <t>fizyka</t>
+        </is>
+      </c>
+      <c r="C19" s="5" t="inlineStr">
+        <is>
+          <t>1.</t>
+        </is>
+      </c>
+      <c r="D19" s="6" t="inlineStr">
+        <is>
+          <t>fizyka</t>
+        </is>
+      </c>
+      <c r="E19" s="6" t="n">
         <v>18</v>
       </c>
     </row>
     <row r="20" ht="14.3" customHeight="1">
-      <c r="A20" s="9" t="n"/>
-      <c r="B20" s="9" t="n"/>
+      <c r="A20" s="4" t="inlineStr">
+        <is>
+          <t>12.</t>
+        </is>
+      </c>
+      <c r="B20" s="4" t="inlineStr">
+        <is>
+          <t>geogr</t>
+        </is>
+      </c>
       <c r="C20" s="4" t="inlineStr">
         <is>
-          <t>4.</t>
+          <t>1.</t>
         </is>
       </c>
       <c r="D20" s="7" t="inlineStr">
         <is>
-          <t>b.h.p-log</t>
+          <t>geogr.r</t>
         </is>
       </c>
       <c r="E20" s="7" t="n">
@@ -1483,66 +1563,66 @@
       </c>
     </row>
     <row r="21" ht="14.3" customHeight="1">
-      <c r="A21" s="5" t="inlineStr">
-        <is>
-          <t>3.</t>
-        </is>
-      </c>
-      <c r="B21" s="5" t="inlineStr">
-        <is>
-          <t>b.i.z</t>
-        </is>
-      </c>
-      <c r="C21" s="5" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D21" s="6" t="inlineStr">
-        <is>
-          <t>b.i.z</t>
-        </is>
-      </c>
-      <c r="E21" s="6" t="n">
+      <c r="A21" s="9" t="n"/>
+      <c r="B21" s="9" t="n"/>
+      <c r="C21" s="4" t="inlineStr">
+        <is>
+          <t>2.</t>
+        </is>
+      </c>
+      <c r="D21" s="7" t="inlineStr">
+        <is>
+          <t>geografia</t>
+        </is>
+      </c>
+      <c r="E21" s="7" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="22" ht="14.3" customHeight="1">
-      <c r="A22" s="4" t="inlineStr">
-        <is>
-          <t>4.</t>
-        </is>
-      </c>
-      <c r="B22" s="4" t="inlineStr">
-        <is>
-          <t>biol</t>
-        </is>
-      </c>
-      <c r="C22" s="4" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D22" s="7" t="inlineStr">
-        <is>
-          <t>biol.r</t>
-        </is>
-      </c>
-      <c r="E22" s="7" t="n">
+      <c r="A22" s="5" t="inlineStr">
+        <is>
+          <t>13.</t>
+        </is>
+      </c>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>h.i.t</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>1.</t>
+        </is>
+      </c>
+      <c r="D22" s="6" t="inlineStr">
+        <is>
+          <t>h.i.t</t>
+        </is>
+      </c>
+      <c r="E22" s="6" t="n">
         <v>21</v>
       </c>
     </row>
     <row r="23" ht="14.3" customHeight="1">
-      <c r="A23" s="8" t="n"/>
-      <c r="B23" s="8" t="n"/>
+      <c r="A23" s="4" t="inlineStr">
+        <is>
+          <t>14.</t>
+        </is>
+      </c>
+      <c r="B23" s="4" t="inlineStr">
+        <is>
+          <t>higiena</t>
+        </is>
+      </c>
       <c r="C23" s="4" t="inlineStr">
         <is>
-          <t>2.</t>
+          <t>1.</t>
         </is>
       </c>
       <c r="D23" s="7" t="inlineStr">
         <is>
-          <t>biol.r-fry</t>
+          <t>higiena</t>
         </is>
       </c>
       <c r="E23" s="7" t="n">
@@ -1550,33 +1630,49 @@
       </c>
     </row>
     <row r="24" ht="14.3" customHeight="1">
-      <c r="A24" s="8" t="n"/>
-      <c r="B24" s="8" t="n"/>
-      <c r="C24" s="4" t="inlineStr">
-        <is>
-          <t>3.</t>
-        </is>
-      </c>
-      <c r="D24" s="7" t="inlineStr">
-        <is>
-          <t>biologia</t>
-        </is>
-      </c>
-      <c r="E24" s="7" t="n">
+      <c r="A24" s="5" t="inlineStr">
+        <is>
+          <t>15.</t>
+        </is>
+      </c>
+      <c r="B24" s="5" t="inlineStr">
+        <is>
+          <t>historia</t>
+        </is>
+      </c>
+      <c r="C24" s="5" t="inlineStr">
+        <is>
+          <t>1.</t>
+        </is>
+      </c>
+      <c r="D24" s="6" t="inlineStr">
+        <is>
+          <t>historia</t>
+        </is>
+      </c>
+      <c r="E24" s="6" t="n">
         <v>23</v>
       </c>
     </row>
     <row r="25" ht="14.3" customHeight="1">
-      <c r="A25" s="8" t="n"/>
-      <c r="B25" s="8" t="n"/>
+      <c r="A25" s="4" t="inlineStr">
+        <is>
+          <t>16.</t>
+        </is>
+      </c>
+      <c r="B25" s="4" t="inlineStr">
+        <is>
+          <t>infor</t>
+        </is>
+      </c>
       <c r="C25" s="4" t="inlineStr">
         <is>
-          <t>4.</t>
+          <t>1.</t>
         </is>
       </c>
       <c r="D25" s="7" t="inlineStr">
         <is>
-          <t>biologia-ek</t>
+          <t>infor</t>
         </is>
       </c>
       <c r="E25" s="7" t="n">
@@ -1584,33 +1680,49 @@
       </c>
     </row>
     <row r="26" ht="14.3" customHeight="1">
-      <c r="A26" s="8" t="n"/>
-      <c r="B26" s="8" t="n"/>
-      <c r="C26" s="4" t="inlineStr">
-        <is>
-          <t>5.</t>
-        </is>
-      </c>
-      <c r="D26" s="7" t="inlineStr">
-        <is>
-          <t>biologia-fry</t>
-        </is>
-      </c>
-      <c r="E26" s="7" t="n">
+      <c r="A26" s="5" t="inlineStr">
+        <is>
+          <t>17.</t>
+        </is>
+      </c>
+      <c r="B26" s="5" t="inlineStr">
+        <is>
+          <t>jęz.polski</t>
+        </is>
+      </c>
+      <c r="C26" s="5" t="inlineStr">
+        <is>
+          <t>1.</t>
+        </is>
+      </c>
+      <c r="D26" s="6" t="inlineStr">
+        <is>
+          <t>jęz.polski</t>
+        </is>
+      </c>
+      <c r="E26" s="6" t="n">
         <v>25</v>
       </c>
     </row>
     <row r="27" ht="14.3" customHeight="1">
-      <c r="A27" s="9" t="n"/>
-      <c r="B27" s="9" t="n"/>
+      <c r="A27" s="4" t="inlineStr">
+        <is>
+          <t>18.</t>
+        </is>
+      </c>
+      <c r="B27" s="4" t="inlineStr">
+        <is>
+          <t>k.p.s</t>
+        </is>
+      </c>
       <c r="C27" s="4" t="inlineStr">
         <is>
-          <t>6.</t>
+          <t>1.</t>
         </is>
       </c>
       <c r="D27" s="7" t="inlineStr">
         <is>
-          <t>biologia-ra</t>
+          <t>k.p.s</t>
         </is>
       </c>
       <c r="E27" s="7" t="n">
@@ -1620,12 +1732,12 @@
     <row r="28" ht="14.3" customHeight="1">
       <c r="A28" s="5" t="inlineStr">
         <is>
-          <t>5.</t>
+          <t>19.</t>
         </is>
       </c>
       <c r="B28" s="5" t="inlineStr">
         <is>
-          <t>chemia</t>
+          <t>mark</t>
         </is>
       </c>
       <c r="C28" s="5" t="inlineStr">
@@ -1635,7 +1747,7 @@
       </c>
       <c r="D28" s="6" t="inlineStr">
         <is>
-          <t>chemia</t>
+          <t>mark</t>
         </is>
       </c>
       <c r="E28" s="6" t="n">
@@ -1643,74 +1755,58 @@
       </c>
     </row>
     <row r="29" ht="14.3" customHeight="1">
-      <c r="A29" s="4" t="inlineStr">
-        <is>
-          <t>6.</t>
-        </is>
-      </c>
-      <c r="B29" s="4" t="inlineStr">
-        <is>
-          <t>dok.pr.tr</t>
-        </is>
-      </c>
-      <c r="C29" s="4" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D29" s="7" t="inlineStr">
-        <is>
-          <t>dok.r.pr.tr-log</t>
-        </is>
-      </c>
-      <c r="E29" s="7" t="n">
+      <c r="A29" s="9" t="n"/>
+      <c r="B29" s="9" t="n"/>
+      <c r="C29" s="5" t="inlineStr">
+        <is>
+          <t>2.</t>
+        </is>
+      </c>
+      <c r="D29" s="6" t="inlineStr">
+        <is>
+          <t>mark.hot</t>
+        </is>
+      </c>
+      <c r="E29" s="6" t="n">
         <v>28</v>
       </c>
     </row>
     <row r="30" ht="14.3" customHeight="1">
-      <c r="A30" s="5" t="inlineStr">
-        <is>
-          <t>7.</t>
-        </is>
-      </c>
-      <c r="B30" s="5" t="inlineStr">
-        <is>
-          <t>dok.zd.gos</t>
-        </is>
-      </c>
-      <c r="C30" s="5" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D30" s="6" t="inlineStr">
-        <is>
-          <t>dok.zd.gos-ek</t>
-        </is>
-      </c>
-      <c r="E30" s="6" t="n">
+      <c r="A30" s="4" t="inlineStr">
+        <is>
+          <t>20.</t>
+        </is>
+      </c>
+      <c r="B30" s="4" t="inlineStr">
+        <is>
+          <t>matem</t>
+        </is>
+      </c>
+      <c r="C30" s="4" t="inlineStr">
+        <is>
+          <t>1.</t>
+        </is>
+      </c>
+      <c r="D30" s="7" t="inlineStr">
+        <is>
+          <t>matem.r</t>
+        </is>
+      </c>
+      <c r="E30" s="7" t="n">
         <v>29</v>
       </c>
     </row>
     <row r="31" ht="14.3" customHeight="1">
-      <c r="A31" s="4" t="inlineStr">
-        <is>
-          <t>8.</t>
-        </is>
-      </c>
-      <c r="B31" s="4" t="inlineStr">
-        <is>
-          <t>dz.wec</t>
-        </is>
-      </c>
+      <c r="A31" s="9" t="n"/>
+      <c r="B31" s="9" t="n"/>
       <c r="C31" s="4" t="inlineStr">
         <is>
-          <t>1.</t>
+          <t>2.</t>
         </is>
       </c>
       <c r="D31" s="7" t="inlineStr">
         <is>
-          <t>dz.w.rec-hot</t>
+          <t>matematyka</t>
         </is>
       </c>
       <c r="E31" s="7" t="n">
@@ -1720,12 +1816,12 @@
     <row r="32" ht="14.3" customHeight="1">
       <c r="A32" s="5" t="inlineStr">
         <is>
-          <t>9.</t>
+          <t>21.</t>
         </is>
       </c>
       <c r="B32" s="5" t="inlineStr">
         <is>
-          <t>e.d.b</t>
+          <t>niem</t>
         </is>
       </c>
       <c r="C32" s="5" t="inlineStr">
@@ -1735,7 +1831,7 @@
       </c>
       <c r="D32" s="6" t="inlineStr">
         <is>
-          <t>e.d.b</t>
+          <t>niem</t>
         </is>
       </c>
       <c r="E32" s="6" t="n">
@@ -1745,12 +1841,12 @@
     <row r="33" ht="14.3" customHeight="1">
       <c r="A33" s="4" t="inlineStr">
         <is>
-          <t>10.</t>
+          <t>22.</t>
         </is>
       </c>
       <c r="B33" s="4" t="inlineStr">
         <is>
-          <t>f.p.gos</t>
+          <t>o.k.i.k</t>
         </is>
       </c>
       <c r="C33" s="4" t="inlineStr">
@@ -1760,7 +1856,7 @@
       </c>
       <c r="D33" s="7" t="inlineStr">
         <is>
-          <t>f.p.gos-ek</t>
+          <t>o.k.i.k</t>
         </is>
       </c>
       <c r="E33" s="7" t="n">
@@ -1770,12 +1866,12 @@
     <row r="34" ht="14.3" customHeight="1">
       <c r="A34" s="5" t="inlineStr">
         <is>
-          <t>11.</t>
+          <t>23.</t>
         </is>
       </c>
       <c r="B34" s="5" t="inlineStr">
         <is>
-          <t>fizyka</t>
+          <t>o.m.z</t>
         </is>
       </c>
       <c r="C34" s="5" t="inlineStr">
@@ -1785,7 +1881,7 @@
       </c>
       <c r="D34" s="6" t="inlineStr">
         <is>
-          <t>fizyka</t>
+          <t>o.m.z</t>
         </is>
       </c>
       <c r="E34" s="6" t="n">
@@ -1795,12 +1891,12 @@
     <row r="35" ht="14.3" customHeight="1">
       <c r="A35" s="4" t="inlineStr">
         <is>
-          <t>12.</t>
+          <t>24.</t>
         </is>
       </c>
       <c r="B35" s="4" t="inlineStr">
         <is>
-          <t>geogr</t>
+          <t>o.p.hot</t>
         </is>
       </c>
       <c r="C35" s="4" t="inlineStr">
@@ -1810,7 +1906,7 @@
       </c>
       <c r="D35" s="7" t="inlineStr">
         <is>
-          <t>geogr.r</t>
+          <t>o.p.hot</t>
         </is>
       </c>
       <c r="E35" s="7" t="n">
@@ -1818,33 +1914,49 @@
       </c>
     </row>
     <row r="36" ht="14.3" customHeight="1">
-      <c r="A36" s="8" t="n"/>
-      <c r="B36" s="8" t="n"/>
-      <c r="C36" s="4" t="inlineStr">
-        <is>
-          <t>2.</t>
-        </is>
-      </c>
-      <c r="D36" s="7" t="inlineStr">
-        <is>
-          <t>geogr.r-ek</t>
-        </is>
-      </c>
-      <c r="E36" s="7" t="n">
+      <c r="A36" s="5" t="inlineStr">
+        <is>
+          <t>25.</t>
+        </is>
+      </c>
+      <c r="B36" s="5" t="inlineStr">
+        <is>
+          <t>o.p.mag</t>
+        </is>
+      </c>
+      <c r="C36" s="5" t="inlineStr">
+        <is>
+          <t>1.</t>
+        </is>
+      </c>
+      <c r="D36" s="6" t="inlineStr">
+        <is>
+          <t>o.p.mag</t>
+        </is>
+      </c>
+      <c r="E36" s="6" t="n">
         <v>35</v>
       </c>
     </row>
     <row r="37" ht="14.3" customHeight="1">
-      <c r="A37" s="8" t="n"/>
-      <c r="B37" s="8" t="n"/>
+      <c r="A37" s="4" t="inlineStr">
+        <is>
+          <t>26.</t>
+        </is>
+      </c>
+      <c r="B37" s="4" t="inlineStr">
+        <is>
+          <t>ob.kon</t>
+        </is>
+      </c>
       <c r="C37" s="4" t="inlineStr">
         <is>
-          <t>3.</t>
+          <t>1.</t>
         </is>
       </c>
       <c r="D37" s="7" t="inlineStr">
         <is>
-          <t>geogr.r-fry</t>
+          <t>ob.kon</t>
         </is>
       </c>
       <c r="E37" s="7" t="n">
@@ -1852,33 +1964,49 @@
       </c>
     </row>
     <row r="38" ht="14.3" customHeight="1">
-      <c r="A38" s="8" t="n"/>
-      <c r="B38" s="8" t="n"/>
-      <c r="C38" s="4" t="inlineStr">
-        <is>
-          <t>4.</t>
-        </is>
-      </c>
-      <c r="D38" s="7" t="inlineStr">
-        <is>
-          <t>geografia</t>
-        </is>
-      </c>
-      <c r="E38" s="7" t="n">
+      <c r="A38" s="5" t="inlineStr">
+        <is>
+          <t>27.</t>
+        </is>
+      </c>
+      <c r="B38" s="5" t="inlineStr">
+        <is>
+          <t>or.proc.tr</t>
+        </is>
+      </c>
+      <c r="C38" s="5" t="inlineStr">
+        <is>
+          <t>1.</t>
+        </is>
+      </c>
+      <c r="D38" s="6" t="inlineStr">
+        <is>
+          <t>or.proc.tr</t>
+        </is>
+      </c>
+      <c r="E38" s="6" t="n">
         <v>37</v>
       </c>
     </row>
     <row r="39" ht="14.3" customHeight="1">
-      <c r="A39" s="8" t="n"/>
-      <c r="B39" s="8" t="n"/>
+      <c r="A39" s="4" t="inlineStr">
+        <is>
+          <t>28.</t>
+        </is>
+      </c>
+      <c r="B39" s="4" t="inlineStr">
+        <is>
+          <t>p.i.d.fry</t>
+        </is>
+      </c>
       <c r="C39" s="4" t="inlineStr">
         <is>
-          <t>5.</t>
+          <t>1.</t>
         </is>
       </c>
       <c r="D39" s="7" t="inlineStr">
         <is>
-          <t>geografia-ek</t>
+          <t>p.i.d.fry</t>
         </is>
       </c>
       <c r="E39" s="7" t="n">
@@ -1886,33 +2014,49 @@
       </c>
     </row>
     <row r="40" ht="14.3" customHeight="1">
-      <c r="A40" s="8" t="n"/>
-      <c r="B40" s="8" t="n"/>
-      <c r="C40" s="4" t="inlineStr">
-        <is>
-          <t>6.</t>
-        </is>
-      </c>
-      <c r="D40" s="7" t="inlineStr">
-        <is>
-          <t>geografia-fry</t>
-        </is>
-      </c>
-      <c r="E40" s="7" t="n">
+      <c r="A40" s="5" t="inlineStr">
+        <is>
+          <t>29.</t>
+        </is>
+      </c>
+      <c r="B40" s="5" t="inlineStr">
+        <is>
+          <t>p.i.w.zap</t>
+        </is>
+      </c>
+      <c r="C40" s="5" t="inlineStr">
+        <is>
+          <t>1.</t>
+        </is>
+      </c>
+      <c r="D40" s="6" t="inlineStr">
+        <is>
+          <t>p.i.w.zap</t>
+        </is>
+      </c>
+      <c r="E40" s="6" t="n">
         <v>39</v>
       </c>
     </row>
     <row r="41" ht="14.3" customHeight="1">
-      <c r="A41" s="9" t="n"/>
-      <c r="B41" s="9" t="n"/>
+      <c r="A41" s="4" t="inlineStr">
+        <is>
+          <t>30.</t>
+        </is>
+      </c>
+      <c r="B41" s="4" t="inlineStr">
+        <is>
+          <t>pl.p.trans</t>
+        </is>
+      </c>
       <c r="C41" s="4" t="inlineStr">
         <is>
-          <t>7.</t>
+          <t>1.</t>
         </is>
       </c>
       <c r="D41" s="7" t="inlineStr">
         <is>
-          <t>geografia-ra</t>
+          <t>pl.p.trans</t>
         </is>
       </c>
       <c r="E41" s="7" t="n">
@@ -1922,12 +2066,12 @@
     <row r="42" ht="14.3" customHeight="1">
       <c r="A42" s="5" t="inlineStr">
         <is>
-          <t>13.</t>
+          <t>31.</t>
         </is>
       </c>
       <c r="B42" s="5" t="inlineStr">
         <is>
-          <t>h.i.t</t>
+          <t>plastyka</t>
         </is>
       </c>
       <c r="C42" s="5" t="inlineStr">
@@ -1937,7 +2081,7 @@
       </c>
       <c r="D42" s="6" t="inlineStr">
         <is>
-          <t>h.i.t</t>
+          <t>plastyka</t>
         </is>
       </c>
       <c r="E42" s="6" t="n">
@@ -1947,12 +2091,12 @@
     <row r="43" ht="14.3" customHeight="1">
       <c r="A43" s="4" t="inlineStr">
         <is>
-          <t>14.</t>
+          <t>32.</t>
         </is>
       </c>
       <c r="B43" s="4" t="inlineStr">
         <is>
-          <t>higiena</t>
+          <t>pod.fry</t>
         </is>
       </c>
       <c r="C43" s="4" t="inlineStr">
@@ -1962,7 +2106,7 @@
       </c>
       <c r="D43" s="7" t="inlineStr">
         <is>
-          <t>higiena-fry</t>
+          <t>pod.fry</t>
         </is>
       </c>
       <c r="E43" s="7" t="n">
@@ -1972,12 +2116,12 @@
     <row r="44" ht="14.3" customHeight="1">
       <c r="A44" s="5" t="inlineStr">
         <is>
-          <t>15.</t>
+          <t>33.</t>
         </is>
       </c>
       <c r="B44" s="5" t="inlineStr">
         <is>
-          <t>historia</t>
+          <t>pod.gas</t>
         </is>
       </c>
       <c r="C44" s="5" t="inlineStr">
@@ -1987,7 +2131,7 @@
       </c>
       <c r="D44" s="6" t="inlineStr">
         <is>
-          <t>historia</t>
+          <t>pod.gas</t>
         </is>
       </c>
       <c r="E44" s="6" t="n">
@@ -1997,12 +2141,12 @@
     <row r="45" ht="14.3" customHeight="1">
       <c r="A45" s="4" t="inlineStr">
         <is>
-          <t>16.</t>
+          <t>34.</t>
         </is>
       </c>
       <c r="B45" s="4" t="inlineStr">
         <is>
-          <t>infor</t>
+          <t>pod.log</t>
         </is>
       </c>
       <c r="C45" s="4" t="inlineStr">
@@ -2012,7 +2156,7 @@
       </c>
       <c r="D45" s="7" t="inlineStr">
         <is>
-          <t>infor</t>
+          <t>pod.log</t>
         </is>
       </c>
       <c r="E45" s="7" t="n">
@@ -2020,33 +2164,49 @@
       </c>
     </row>
     <row r="46" ht="14.3" customHeight="1">
-      <c r="A46" s="8" t="n"/>
-      <c r="B46" s="8" t="n"/>
-      <c r="C46" s="4" t="inlineStr">
-        <is>
-          <t>2.</t>
-        </is>
-      </c>
-      <c r="D46" s="7" t="inlineStr">
-        <is>
-          <t>infor-1/2</t>
-        </is>
-      </c>
-      <c r="E46" s="7" t="n">
+      <c r="A46" s="5" t="inlineStr">
+        <is>
+          <t>35.</t>
+        </is>
+      </c>
+      <c r="B46" s="5" t="inlineStr">
+        <is>
+          <t>pod.prz</t>
+        </is>
+      </c>
+      <c r="C46" s="5" t="inlineStr">
+        <is>
+          <t>1.</t>
+        </is>
+      </c>
+      <c r="D46" s="6" t="inlineStr">
+        <is>
+          <t>pod.prz</t>
+        </is>
+      </c>
+      <c r="E46" s="6" t="n">
         <v>45</v>
       </c>
     </row>
     <row r="47" ht="14.3" customHeight="1">
-      <c r="A47" s="8" t="n"/>
-      <c r="B47" s="8" t="n"/>
+      <c r="A47" s="4" t="inlineStr">
+        <is>
+          <t>36.</t>
+        </is>
+      </c>
+      <c r="B47" s="4" t="inlineStr">
+        <is>
+          <t>pod.stat</t>
+        </is>
+      </c>
       <c r="C47" s="4" t="inlineStr">
         <is>
-          <t>3.</t>
+          <t>1.</t>
         </is>
       </c>
       <c r="D47" s="7" t="inlineStr">
         <is>
-          <t>infor-2/2</t>
+          <t>pod.stat</t>
         </is>
       </c>
       <c r="E47" s="7" t="n">
@@ -2054,33 +2214,49 @@
       </c>
     </row>
     <row r="48" ht="14.3" customHeight="1">
-      <c r="A48" s="8" t="n"/>
-      <c r="B48" s="8" t="n"/>
-      <c r="C48" s="4" t="inlineStr">
-        <is>
-          <t>4.</t>
-        </is>
-      </c>
-      <c r="D48" s="7" t="inlineStr">
-        <is>
-          <t>infor-ek</t>
-        </is>
-      </c>
-      <c r="E48" s="7" t="n">
+      <c r="A48" s="5" t="inlineStr">
+        <is>
+          <t>37.</t>
+        </is>
+      </c>
+      <c r="B48" s="5" t="inlineStr">
+        <is>
+          <t>pod.żyw</t>
+        </is>
+      </c>
+      <c r="C48" s="5" t="inlineStr">
+        <is>
+          <t>1.</t>
+        </is>
+      </c>
+      <c r="D48" s="6" t="inlineStr">
+        <is>
+          <t>pod.żyw</t>
+        </is>
+      </c>
+      <c r="E48" s="6" t="n">
         <v>47</v>
       </c>
     </row>
     <row r="49" ht="14.3" customHeight="1">
-      <c r="A49" s="8" t="n"/>
-      <c r="B49" s="8" t="n"/>
+      <c r="A49" s="4" t="inlineStr">
+        <is>
+          <t>38.</t>
+        </is>
+      </c>
+      <c r="B49" s="4" t="inlineStr">
+        <is>
+          <t>pr.est</t>
+        </is>
+      </c>
       <c r="C49" s="4" t="inlineStr">
         <is>
-          <t>5.</t>
+          <t>1.</t>
         </is>
       </c>
       <c r="D49" s="7" t="inlineStr">
         <is>
-          <t>infor-fry</t>
+          <t>pr.est</t>
         </is>
       </c>
       <c r="E49" s="7" t="n">
@@ -2088,84 +2264,100 @@
       </c>
     </row>
     <row r="50" ht="14.3" customHeight="1">
-      <c r="A50" s="8" t="n"/>
-      <c r="B50" s="8" t="n"/>
-      <c r="C50" s="4" t="inlineStr">
-        <is>
-          <t>6.</t>
-        </is>
-      </c>
-      <c r="D50" s="7" t="inlineStr">
-        <is>
-          <t>infor-gas</t>
-        </is>
-      </c>
-      <c r="E50" s="7" t="n">
+      <c r="A50" s="5" t="inlineStr">
+        <is>
+          <t>39.</t>
+        </is>
+      </c>
+      <c r="B50" s="5" t="inlineStr">
+        <is>
+          <t>pr.fry</t>
+        </is>
+      </c>
+      <c r="C50" s="5" t="inlineStr">
+        <is>
+          <t>1.</t>
+        </is>
+      </c>
+      <c r="D50" s="6" t="inlineStr">
+        <is>
+          <t>pr.fry</t>
+        </is>
+      </c>
+      <c r="E50" s="6" t="n">
         <v>49</v>
       </c>
     </row>
     <row r="51" ht="14.3" customHeight="1">
       <c r="A51" s="8" t="n"/>
       <c r="B51" s="8" t="n"/>
-      <c r="C51" s="4" t="inlineStr">
-        <is>
-          <t>7.</t>
-        </is>
-      </c>
-      <c r="D51" s="7" t="inlineStr">
-        <is>
-          <t>infor-hot</t>
-        </is>
-      </c>
-      <c r="E51" s="7" t="n">
+      <c r="C51" s="5" t="inlineStr">
+        <is>
+          <t>2.</t>
+        </is>
+      </c>
+      <c r="D51" s="6" t="inlineStr">
+        <is>
+          <t>pr.fry-M</t>
+        </is>
+      </c>
+      <c r="E51" s="6" t="n">
         <v>50</v>
       </c>
     </row>
     <row r="52" ht="14.3" customHeight="1">
       <c r="A52" s="8" t="n"/>
       <c r="B52" s="8" t="n"/>
-      <c r="C52" s="4" t="inlineStr">
-        <is>
-          <t>8.</t>
-        </is>
-      </c>
-      <c r="D52" s="7" t="inlineStr">
-        <is>
-          <t>infor-j1</t>
-        </is>
-      </c>
-      <c r="E52" s="7" t="n">
+      <c r="C52" s="5" t="inlineStr">
+        <is>
+          <t>3.</t>
+        </is>
+      </c>
+      <c r="D52" s="6" t="inlineStr">
+        <is>
+          <t>pr.fry.dam</t>
+        </is>
+      </c>
+      <c r="E52" s="6" t="n">
         <v>51</v>
       </c>
     </row>
     <row r="53" ht="14.3" customHeight="1">
-      <c r="A53" s="8" t="n"/>
-      <c r="B53" s="8" t="n"/>
-      <c r="C53" s="4" t="inlineStr">
-        <is>
-          <t>9.</t>
-        </is>
-      </c>
-      <c r="D53" s="7" t="inlineStr">
-        <is>
-          <t>infor-j2</t>
-        </is>
-      </c>
-      <c r="E53" s="7" t="n">
+      <c r="A53" s="9" t="n"/>
+      <c r="B53" s="9" t="n"/>
+      <c r="C53" s="5" t="inlineStr">
+        <is>
+          <t>4.</t>
+        </is>
+      </c>
+      <c r="D53" s="6" t="inlineStr">
+        <is>
+          <t>pr.fry.men</t>
+        </is>
+      </c>
+      <c r="E53" s="6" t="n">
         <v>52</v>
       </c>
     </row>
     <row r="54" ht="14.3" customHeight="1">
-      <c r="A54" s="8" t="n"/>
-      <c r="B54" s="8" t="n"/>
+      <c r="A54" s="4" t="inlineStr">
+        <is>
+          <t>40.</t>
+        </is>
+      </c>
+      <c r="B54" s="4" t="inlineStr">
+        <is>
+          <t>pr.gas</t>
+        </is>
+      </c>
       <c r="C54" s="4" t="inlineStr">
         <is>
-          <t>10.</t>
+          <t>1.</t>
         </is>
       </c>
       <c r="D54" s="7" t="inlineStr">
         <is>
-          <t>infor-log</t>
+          <t>pr.gas</t>
         </is>
       </c>
       <c r="E54" s="7" t="n">
@@ -2173,58 +2365,74 @@
       </c>
     </row>
     <row r="55" ht="14.3" customHeight="1">
-      <c r="A55" s="9" t="n"/>
-      <c r="B55" s="9" t="n"/>
-      <c r="C55" s="4" t="inlineStr">
-        <is>
-          <t>11.</t>
-        </is>
-      </c>
-      <c r="D55" s="7" t="inlineStr">
-        <is>
-          <t>infor-ra</t>
-        </is>
-      </c>
-      <c r="E55" s="7" t="n">
+      <c r="A55" s="5" t="inlineStr">
+        <is>
+          <t>41.</t>
+        </is>
+      </c>
+      <c r="B55" s="5" t="inlineStr">
+        <is>
+          <t>pr.hot</t>
+        </is>
+      </c>
+      <c r="C55" s="5" t="inlineStr">
+        <is>
+          <t>1.</t>
+        </is>
+      </c>
+      <c r="D55" s="6" t="inlineStr">
+        <is>
+          <t>pr.hot</t>
+        </is>
+      </c>
+      <c r="E55" s="6" t="n">
         <v>54</v>
       </c>
     </row>
     <row r="56" ht="14.3" customHeight="1">
-      <c r="A56" s="5" t="inlineStr">
-        <is>
-          <t>17.</t>
-        </is>
-      </c>
-      <c r="B56" s="5" t="inlineStr">
-        <is>
-          <t>jęz.polski</t>
-        </is>
-      </c>
-      <c r="C56" s="5" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D56" s="6" t="inlineStr">
-        <is>
-          <t>jęz.polski</t>
-        </is>
-      </c>
-      <c r="E56" s="6" t="n">
+      <c r="A56" s="4" t="inlineStr">
+        <is>
+          <t>42.</t>
+        </is>
+      </c>
+      <c r="B56" s="4" t="inlineStr">
+        <is>
+          <t>pr.k.p.fry</t>
+        </is>
+      </c>
+      <c r="C56" s="4" t="inlineStr">
+        <is>
+          <t>1.</t>
+        </is>
+      </c>
+      <c r="D56" s="7" t="inlineStr">
+        <is>
+          <t>pr.k.p.fry</t>
+        </is>
+      </c>
+      <c r="E56" s="7" t="n">
         <v>55</v>
       </c>
     </row>
     <row r="57" ht="14.3" customHeight="1">
-      <c r="A57" s="9" t="n"/>
-      <c r="B57" s="9" t="n"/>
+      <c r="A57" s="5" t="inlineStr">
+        <is>
+          <t>43.</t>
+        </is>
+      </c>
+      <c r="B57" s="5" t="inlineStr">
+        <is>
+          <t>pr.kosm</t>
+        </is>
+      </c>
       <c r="C57" s="5" t="inlineStr">
         <is>
-          <t>2.</t>
+          <t>1.</t>
         </is>
       </c>
       <c r="D57" s="6" t="inlineStr">
         <is>
-          <t>jęz.polski-pol</t>
+          <t>pr.kosm</t>
         </is>
       </c>
       <c r="E57" s="6" t="n">
@@ -2234,12 +2442,12 @@
     <row r="58" ht="14.3" customHeight="1">
       <c r="A58" s="4" t="inlineStr">
         <is>
-          <t>18.</t>
+          <t>44.</t>
         </is>
       </c>
       <c r="B58" s="4" t="inlineStr">
         <is>
-          <t>k.p.s</t>
+          <t>pr.ob.inf</t>
         </is>
       </c>
       <c r="C58" s="4" t="inlineStr">
@@ -2249,7 +2457,7 @@
       </c>
       <c r="D58" s="7" t="inlineStr">
         <is>
-          <t>k.p.s</t>
+          <t>pr.ob.inf</t>
         </is>
       </c>
       <c r="E58" s="7" t="n">
@@ -2257,33 +2465,49 @@
       </c>
     </row>
     <row r="59" ht="14.3" customHeight="1">
-      <c r="A59" s="8" t="n"/>
-      <c r="B59" s="8" t="n"/>
-      <c r="C59" s="4" t="inlineStr">
-        <is>
-          <t>2.</t>
-        </is>
-      </c>
-      <c r="D59" s="7" t="inlineStr">
-        <is>
-          <t>k.p.s-fry</t>
-        </is>
-      </c>
-      <c r="E59" s="7" t="n">
+      <c r="A59" s="5" t="inlineStr">
+        <is>
+          <t>45.</t>
+        </is>
+      </c>
+      <c r="B59" s="5" t="inlineStr">
+        <is>
+          <t>pr.ob.kon</t>
+        </is>
+      </c>
+      <c r="C59" s="5" t="inlineStr">
+        <is>
+          <t>1.</t>
+        </is>
+      </c>
+      <c r="D59" s="6" t="inlineStr">
+        <is>
+          <t>pr.ob.kon</t>
+        </is>
+      </c>
+      <c r="E59" s="6" t="n">
         <v>58</v>
       </c>
     </row>
     <row r="60" ht="14.3" customHeight="1">
-      <c r="A60" s="8" t="n"/>
-      <c r="B60" s="8" t="n"/>
+      <c r="A60" s="4" t="inlineStr">
+        <is>
+          <t>46.</t>
+        </is>
+      </c>
+      <c r="B60" s="4" t="inlineStr">
+        <is>
+          <t>pr.p.est</t>
+        </is>
+      </c>
       <c r="C60" s="4" t="inlineStr">
         <is>
-          <t>3.</t>
+          <t>1.</t>
         </is>
       </c>
       <c r="D60" s="7" t="inlineStr">
         <is>
-          <t>k.p.s-gas</t>
+          <t>pr.p.est</t>
         </is>
       </c>
       <c r="E60" s="7" t="n">
@@ -2291,58 +2515,74 @@
       </c>
     </row>
     <row r="61" ht="14.3" customHeight="1">
-      <c r="A61" s="9" t="n"/>
-      <c r="B61" s="9" t="n"/>
-      <c r="C61" s="4" t="inlineStr">
-        <is>
-          <t>4.</t>
-        </is>
-      </c>
-      <c r="D61" s="7" t="inlineStr">
-        <is>
-          <t>k.p.s-log</t>
-        </is>
-      </c>
-      <c r="E61" s="7" t="n">
+      <c r="A61" s="5" t="inlineStr">
+        <is>
+          <t>47.</t>
+        </is>
+      </c>
+      <c r="B61" s="5" t="inlineStr">
+        <is>
+          <t>pr.rach</t>
+        </is>
+      </c>
+      <c r="C61" s="5" t="inlineStr">
+        <is>
+          <t>1.</t>
+        </is>
+      </c>
+      <c r="D61" s="6" t="inlineStr">
+        <is>
+          <t>pr.rach</t>
+        </is>
+      </c>
+      <c r="E61" s="6" t="n">
         <v>60</v>
       </c>
     </row>
     <row r="62" ht="14.3" customHeight="1">
-      <c r="A62" s="5" t="inlineStr">
-        <is>
-          <t>19.</t>
-        </is>
-      </c>
-      <c r="B62" s="5" t="inlineStr">
-        <is>
-          <t>mark</t>
-        </is>
-      </c>
-      <c r="C62" s="5" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D62" s="6" t="inlineStr">
-        <is>
-          <t>mark-ek</t>
-        </is>
-      </c>
-      <c r="E62" s="6" t="n">
+      <c r="A62" s="4" t="inlineStr">
+        <is>
+          <t>48.</t>
+        </is>
+      </c>
+      <c r="B62" s="4" t="inlineStr">
+        <is>
+          <t>pr.s.k</t>
+        </is>
+      </c>
+      <c r="C62" s="4" t="inlineStr">
+        <is>
+          <t>1.</t>
+        </is>
+      </c>
+      <c r="D62" s="7" t="inlineStr">
+        <is>
+          <t>pr.s.k-pła</t>
+        </is>
+      </c>
+      <c r="E62" s="7" t="n">
         <v>61</v>
       </c>
     </row>
     <row r="63" ht="14.3" customHeight="1">
-      <c r="A63" s="9" t="n"/>
-      <c r="B63" s="9" t="n"/>
+      <c r="A63" s="5" t="inlineStr">
+        <is>
+          <t>49.</t>
+        </is>
+      </c>
+      <c r="B63" s="5" t="inlineStr">
+        <is>
+          <t>pr.t.biu</t>
+        </is>
+      </c>
       <c r="C63" s="5" t="inlineStr">
         <is>
-          <t>2.</t>
+          <t>1.</t>
         </is>
       </c>
       <c r="D63" s="6" t="inlineStr">
         <is>
-          <t>mark.hot</t>
+          <t>pr.t.biu</t>
         </is>
       </c>
       <c r="E63" s="6" t="n">
@@ -2352,12 +2592,12 @@
     <row r="64" ht="14.3" customHeight="1">
       <c r="A64" s="4" t="inlineStr">
         <is>
-          <t>20.</t>
+          <t>50.</t>
         </is>
       </c>
       <c r="B64" s="4" t="inlineStr">
         <is>
-          <t>matem</t>
+          <t>pr.wyp.tech</t>
         </is>
       </c>
       <c r="C64" s="4" t="inlineStr">
@@ -2367,7 +2607,7 @@
       </c>
       <c r="D64" s="7" t="inlineStr">
         <is>
-          <t>matem.r</t>
+          <t>pr.wyp.tech</t>
         </is>
       </c>
       <c r="E64" s="7" t="n">
@@ -2375,33 +2615,49 @@
       </c>
     </row>
     <row r="65" ht="14.3" customHeight="1">
-      <c r="A65" s="8" t="n"/>
-      <c r="B65" s="8" t="n"/>
-      <c r="C65" s="4" t="inlineStr">
-        <is>
-          <t>2.</t>
-        </is>
-      </c>
-      <c r="D65" s="7" t="inlineStr">
-        <is>
-          <t>matematyka</t>
-        </is>
-      </c>
-      <c r="E65" s="7" t="n">
+      <c r="A65" s="5" t="inlineStr">
+        <is>
+          <t>51.</t>
+        </is>
+      </c>
+      <c r="B65" s="5" t="inlineStr">
+        <is>
+          <t>pra.d.g</t>
+        </is>
+      </c>
+      <c r="C65" s="5" t="inlineStr">
+        <is>
+          <t>1.</t>
+        </is>
+      </c>
+      <c r="D65" s="6" t="inlineStr">
+        <is>
+          <t>pra.d.g</t>
+        </is>
+      </c>
+      <c r="E65" s="6" t="n">
         <v>64</v>
       </c>
     </row>
     <row r="66" ht="14.3" customHeight="1">
-      <c r="A66" s="9" t="n"/>
-      <c r="B66" s="9" t="n"/>
+      <c r="A66" s="4" t="inlineStr">
+        <is>
+          <t>52.</t>
+        </is>
+      </c>
+      <c r="B66" s="4" t="inlineStr">
+        <is>
+          <t>pro.gos.fin</t>
+        </is>
+      </c>
       <c r="C66" s="4" t="inlineStr">
         <is>
-          <t>3.</t>
+          <t>1.</t>
         </is>
       </c>
       <c r="D66" s="7" t="inlineStr">
         <is>
-          <t>matematyka-mat</t>
+          <t>pro.gos.fin</t>
         </is>
       </c>
       <c r="E66" s="7" t="n">
@@ -2411,12 +2667,12 @@
     <row r="67" ht="14.3" customHeight="1">
       <c r="A67" s="5" t="inlineStr">
         <is>
-          <t>21.</t>
+          <t>53.</t>
         </is>
       </c>
       <c r="B67" s="5" t="inlineStr">
         <is>
-          <t>niem</t>
+          <t>przech.zap</t>
         </is>
       </c>
       <c r="C67" s="5" t="inlineStr">
@@ -2426,7 +2682,7 @@
       </c>
       <c r="D67" s="6" t="inlineStr">
         <is>
-          <t>niem-fry</t>
+          <t>przech.zap</t>
         </is>
       </c>
       <c r="E67" s="6" t="n">
@@ -2434,33 +2690,49 @@
       </c>
     </row>
     <row r="68" ht="14.3" customHeight="1">
-      <c r="A68" s="8" t="n"/>
-      <c r="B68" s="8" t="n"/>
-      <c r="C68" s="5" t="inlineStr">
-        <is>
-          <t>2.</t>
-        </is>
-      </c>
-      <c r="D68" s="6" t="inlineStr">
-        <is>
-          <t>niem-gas</t>
-        </is>
-      </c>
-      <c r="E68" s="6" t="n">
+      <c r="A68" s="4" t="inlineStr">
+        <is>
+          <t>54.</t>
+        </is>
+      </c>
+      <c r="B68" s="4" t="inlineStr">
+        <is>
+          <t>rach.fin</t>
+        </is>
+      </c>
+      <c r="C68" s="4" t="inlineStr">
+        <is>
+          <t>1.</t>
+        </is>
+      </c>
+      <c r="D68" s="7" t="inlineStr">
+        <is>
+          <t>rach.fin</t>
+        </is>
+      </c>
+      <c r="E68" s="7" t="n">
         <v>67</v>
       </c>
     </row>
     <row r="69" ht="14.3" customHeight="1">
-      <c r="A69" s="8" t="n"/>
-      <c r="B69" s="8" t="n"/>
+      <c r="A69" s="5" t="inlineStr">
+        <is>
+          <t>55.</t>
+        </is>
+      </c>
+      <c r="B69" s="5" t="inlineStr">
+        <is>
+          <t>religia</t>
+        </is>
+      </c>
       <c r="C69" s="5" t="inlineStr">
         <is>
-          <t>3.</t>
+          <t>1.</t>
         </is>
       </c>
       <c r="D69" s="6" t="inlineStr">
         <is>
-          <t>niem-log</t>
+          <t>religia</t>
         </is>
       </c>
       <c r="E69" s="6" t="n">
@@ -2468,83 +2740,99 @@
       </c>
     </row>
     <row r="70" ht="14.3" customHeight="1">
-      <c r="A70" s="9" t="n"/>
-      <c r="B70" s="9" t="n"/>
-      <c r="C70" s="5" t="inlineStr">
-        <is>
-          <t>4.</t>
-        </is>
-      </c>
-      <c r="D70" s="6" t="inlineStr">
-        <is>
-          <t>niem-ra</t>
-        </is>
-      </c>
-      <c r="E70" s="6" t="n">
+      <c r="A70" s="4" t="inlineStr">
+        <is>
+          <t>56.</t>
+        </is>
+      </c>
+      <c r="B70" s="4" t="inlineStr">
+        <is>
+          <t>stat</t>
+        </is>
+      </c>
+      <c r="C70" s="4" t="inlineStr">
+        <is>
+          <t>1.</t>
+        </is>
+      </c>
+      <c r="D70" s="7" t="inlineStr">
+        <is>
+          <t>stat</t>
+        </is>
+      </c>
+      <c r="E70" s="7" t="n">
         <v>69</v>
       </c>
     </row>
     <row r="71" ht="14.3" customHeight="1">
-      <c r="A71" s="4" t="inlineStr">
-        <is>
-          <t>22.</t>
-        </is>
-      </c>
-      <c r="B71" s="4" t="inlineStr">
-        <is>
-          <t>o.k.i.k</t>
-        </is>
-      </c>
-      <c r="C71" s="4" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D71" s="7" t="inlineStr">
-        <is>
-          <t>o.k.i.k-log</t>
-        </is>
-      </c>
-      <c r="E71" s="7" t="n">
+      <c r="A71" s="5" t="inlineStr">
+        <is>
+          <t>57.</t>
+        </is>
+      </c>
+      <c r="B71" s="5" t="inlineStr">
+        <is>
+          <t>t.fry</t>
+        </is>
+      </c>
+      <c r="C71" s="5" t="inlineStr">
+        <is>
+          <t>1.</t>
+        </is>
+      </c>
+      <c r="D71" s="6" t="inlineStr">
+        <is>
+          <t>t.fry</t>
+        </is>
+      </c>
+      <c r="E71" s="6" t="n">
         <v>70</v>
       </c>
     </row>
     <row r="72" ht="14.3" customHeight="1">
-      <c r="A72" s="5" t="inlineStr">
-        <is>
-          <t>23.</t>
-        </is>
-      </c>
-      <c r="B72" s="5" t="inlineStr">
-        <is>
-          <t>o.m.z</t>
-        </is>
-      </c>
-      <c r="C72" s="5" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D72" s="6" t="inlineStr">
-        <is>
-          <t>o.m.z</t>
-        </is>
-      </c>
-      <c r="E72" s="6" t="n">
+      <c r="A72" s="4" t="inlineStr">
+        <is>
+          <t>58.</t>
+        </is>
+      </c>
+      <c r="B72" s="4" t="inlineStr">
+        <is>
+          <t>us.w.gas</t>
+        </is>
+      </c>
+      <c r="C72" s="4" t="inlineStr">
+        <is>
+          <t>1.</t>
+        </is>
+      </c>
+      <c r="D72" s="7" t="inlineStr">
+        <is>
+          <t>us.w.gas</t>
+        </is>
+      </c>
+      <c r="E72" s="7" t="n">
         <v>71</v>
       </c>
     </row>
     <row r="73" ht="14.3" customHeight="1">
-      <c r="A73" s="8" t="n"/>
-      <c r="B73" s="8" t="n"/>
+      <c r="A73" s="5" t="inlineStr">
+        <is>
+          <t>59.</t>
+        </is>
+      </c>
+      <c r="B73" s="5" t="inlineStr">
+        <is>
+          <t>w.f</t>
+        </is>
+      </c>
       <c r="C73" s="5" t="inlineStr">
         <is>
-          <t>2.</t>
+          <t>1.</t>
         </is>
       </c>
       <c r="D73" s="6" t="inlineStr">
         <is>
-          <t>o.m.z-gas</t>
+          <t>w.f</t>
         </is>
       </c>
       <c r="E73" s="6" t="n">
@@ -2552,108 +2840,124 @@
       </c>
     </row>
     <row r="74" ht="14.3" customHeight="1">
-      <c r="A74" s="9" t="n"/>
-      <c r="B74" s="9" t="n"/>
-      <c r="C74" s="5" t="inlineStr">
-        <is>
-          <t>3.</t>
-        </is>
-      </c>
-      <c r="D74" s="6" t="inlineStr">
-        <is>
-          <t>o.m.z-log</t>
-        </is>
-      </c>
-      <c r="E74" s="6" t="n">
+      <c r="A74" s="4" t="inlineStr">
+        <is>
+          <t>60.</t>
+        </is>
+      </c>
+      <c r="B74" s="4" t="inlineStr">
+        <is>
+          <t>w.o.s</t>
+        </is>
+      </c>
+      <c r="C74" s="4" t="inlineStr">
+        <is>
+          <t>1.</t>
+        </is>
+      </c>
+      <c r="D74" s="7" t="inlineStr">
+        <is>
+          <t>w.o.s</t>
+        </is>
+      </c>
+      <c r="E74" s="7" t="n">
         <v>73</v>
       </c>
     </row>
     <row r="75" ht="14.3" customHeight="1">
-      <c r="A75" s="4" t="inlineStr">
-        <is>
-          <t>24.</t>
-        </is>
-      </c>
-      <c r="B75" s="4" t="inlineStr">
-        <is>
-          <t>o.p.hot</t>
-        </is>
-      </c>
-      <c r="C75" s="4" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D75" s="7" t="inlineStr">
-        <is>
-          <t>o.p.hot</t>
-        </is>
-      </c>
-      <c r="E75" s="7" t="n">
+      <c r="A75" s="5" t="inlineStr">
+        <is>
+          <t>61.</t>
+        </is>
+      </c>
+      <c r="B75" s="5" t="inlineStr">
+        <is>
+          <t>wło</t>
+        </is>
+      </c>
+      <c r="C75" s="5" t="inlineStr">
+        <is>
+          <t>1.</t>
+        </is>
+      </c>
+      <c r="D75" s="6" t="inlineStr">
+        <is>
+          <t>wło</t>
+        </is>
+      </c>
+      <c r="E75" s="6" t="n">
         <v>74</v>
       </c>
     </row>
     <row r="76" ht="14.3" customHeight="1">
-      <c r="A76" s="5" t="inlineStr">
-        <is>
-          <t>25.</t>
-        </is>
-      </c>
-      <c r="B76" s="5" t="inlineStr">
-        <is>
-          <t>o.p.mag</t>
-        </is>
-      </c>
-      <c r="C76" s="5" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D76" s="6" t="inlineStr">
-        <is>
-          <t>o.p.mag-log</t>
-        </is>
-      </c>
-      <c r="E76" s="6" t="n">
+      <c r="A76" s="4" t="inlineStr">
+        <is>
+          <t>62.</t>
+        </is>
+      </c>
+      <c r="B76" s="4" t="inlineStr">
+        <is>
+          <t>z.r.wło</t>
+        </is>
+      </c>
+      <c r="C76" s="4" t="inlineStr">
+        <is>
+          <t>1.</t>
+        </is>
+      </c>
+      <c r="D76" s="7" t="inlineStr">
+        <is>
+          <t>z.r.wło</t>
+        </is>
+      </c>
+      <c r="E76" s="7" t="n">
         <v>75</v>
       </c>
     </row>
     <row r="77" ht="14.3" customHeight="1">
-      <c r="A77" s="4" t="inlineStr">
-        <is>
-          <t>26.</t>
-        </is>
-      </c>
-      <c r="B77" s="4" t="inlineStr">
-        <is>
-          <t>ob.kon</t>
-        </is>
-      </c>
-      <c r="C77" s="4" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D77" s="7" t="inlineStr">
-        <is>
-          <t>ob.kon</t>
-        </is>
-      </c>
-      <c r="E77" s="7" t="n">
+      <c r="A77" s="5" t="inlineStr">
+        <is>
+          <t>63.</t>
+        </is>
+      </c>
+      <c r="B77" s="5" t="inlineStr">
+        <is>
+          <t>z.z.w</t>
+        </is>
+      </c>
+      <c r="C77" s="5" t="inlineStr">
+        <is>
+          <t>1.</t>
+        </is>
+      </c>
+      <c r="D77" s="6" t="inlineStr">
+        <is>
+          <t>z.z.w</t>
+        </is>
+      </c>
+      <c r="E77" s="6" t="n">
         <v>76</v>
       </c>
     </row>
     <row r="78" ht="14.3" customHeight="1">
-      <c r="A78" s="9" t="n"/>
-      <c r="B78" s="9" t="n"/>
+      <c r="A78" s="4" t="inlineStr">
+        <is>
+          <t>64.</t>
+        </is>
+      </c>
+      <c r="B78" s="4" t="inlineStr">
+        <is>
+          <t>zab.maj</t>
+        </is>
+      </c>
       <c r="C78" s="4" t="inlineStr">
         <is>
-          <t>2.</t>
+          <t>1.</t>
         </is>
       </c>
       <c r="D78" s="7" t="inlineStr">
         <is>
-          <t>ob.kon-gas</t>
+          <t>zab.maj</t>
         </is>
       </c>
       <c r="E78" s="7" t="n">
@@ -2663,12 +2967,12 @@
     <row r="79" ht="14.3" customHeight="1">
       <c r="A79" s="5" t="inlineStr">
         <is>
-          <t>27.</t>
+          <t>65.</t>
         </is>
       </c>
       <c r="B79" s="5" t="inlineStr">
         <is>
-          <t>or.proc.tr</t>
+          <t>zaj.sport</t>
         </is>
       </c>
       <c r="C79" s="5" t="inlineStr">
@@ -2678,1451 +2982,27 @@
       </c>
       <c r="D79" s="6" t="inlineStr">
         <is>
-          <t>or.proc.tr-log</t>
+          <t>zaj.sport</t>
         </is>
       </c>
       <c r="E79" s="6" t="n">
         <v>78</v>
       </c>
     </row>
-    <row r="80" ht="14.3" customHeight="1">
-      <c r="A80" s="4" t="inlineStr">
-        <is>
-          <t>28.</t>
-        </is>
-      </c>
-      <c r="B80" s="4" t="inlineStr">
-        <is>
-          <t>p.i.d.fry</t>
-        </is>
-      </c>
-      <c r="C80" s="4" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D80" s="7" t="inlineStr">
-        <is>
-          <t>p.i.d.fry-fry</t>
-        </is>
-      </c>
-      <c r="E80" s="7" t="n">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="81" ht="14.3" customHeight="1">
-      <c r="A81" s="5" t="inlineStr">
-        <is>
-          <t>29.</t>
-        </is>
-      </c>
-      <c r="B81" s="5" t="inlineStr">
-        <is>
-          <t>p.i.w.zap</t>
-        </is>
-      </c>
-      <c r="C81" s="5" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D81" s="6" t="inlineStr">
-        <is>
-          <t>p.i.w.zap-log</t>
-        </is>
-      </c>
-      <c r="E81" s="6" t="n">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="82" ht="14.3" customHeight="1">
-      <c r="A82" s="4" t="inlineStr">
-        <is>
-          <t>30.</t>
-        </is>
-      </c>
-      <c r="B82" s="4" t="inlineStr">
-        <is>
-          <t>pl.p.trans</t>
-        </is>
-      </c>
-      <c r="C82" s="4" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D82" s="7" t="inlineStr">
-        <is>
-          <t>pl.p.trans</t>
-        </is>
-      </c>
-      <c r="E82" s="7" t="n">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="83" ht="14.3" customHeight="1">
-      <c r="A83" s="9" t="n"/>
-      <c r="B83" s="9" t="n"/>
-      <c r="C83" s="4" t="inlineStr">
-        <is>
-          <t>2.</t>
-        </is>
-      </c>
-      <c r="D83" s="7" t="inlineStr">
-        <is>
-          <t>pl.p.trans-log</t>
-        </is>
-      </c>
-      <c r="E83" s="7" t="n">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="84" ht="14.3" customHeight="1">
-      <c r="A84" s="5" t="inlineStr">
-        <is>
-          <t>31.</t>
-        </is>
-      </c>
-      <c r="B84" s="5" t="inlineStr">
-        <is>
-          <t>plastyka</t>
-        </is>
-      </c>
-      <c r="C84" s="5" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D84" s="6" t="inlineStr">
-        <is>
-          <t>plastyka</t>
-        </is>
-      </c>
-      <c r="E84" s="6" t="n">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="85" ht="14.3" customHeight="1">
-      <c r="A85" s="4" t="inlineStr">
-        <is>
-          <t>32.</t>
-        </is>
-      </c>
-      <c r="B85" s="4" t="inlineStr">
-        <is>
-          <t>pod.fry</t>
-        </is>
-      </c>
-      <c r="C85" s="4" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D85" s="7" t="inlineStr">
-        <is>
-          <t>pod.fry-fry</t>
-        </is>
-      </c>
-      <c r="E85" s="7" t="n">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="86" ht="14.3" customHeight="1">
-      <c r="A86" s="5" t="inlineStr">
-        <is>
-          <t>33.</t>
-        </is>
-      </c>
-      <c r="B86" s="5" t="inlineStr">
-        <is>
-          <t>pod.gas</t>
-        </is>
-      </c>
-      <c r="C86" s="5" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D86" s="6" t="inlineStr">
-        <is>
-          <t>pod.gas</t>
-        </is>
-      </c>
-      <c r="E86" s="6" t="n">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="87" ht="14.3" customHeight="1">
-      <c r="A87" s="9" t="n"/>
-      <c r="B87" s="9" t="n"/>
-      <c r="C87" s="5" t="inlineStr">
-        <is>
-          <t>2.</t>
-        </is>
-      </c>
-      <c r="D87" s="6" t="inlineStr">
-        <is>
-          <t>pod.gas-gas</t>
-        </is>
-      </c>
-      <c r="E87" s="6" t="n">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="88" ht="14.3" customHeight="1">
-      <c r="A88" s="4" t="inlineStr">
-        <is>
-          <t>34.</t>
-        </is>
-      </c>
-      <c r="B88" s="4" t="inlineStr">
-        <is>
-          <t>pod.log</t>
-        </is>
-      </c>
-      <c r="C88" s="4" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D88" s="7" t="inlineStr">
-        <is>
-          <t>pod.log</t>
-        </is>
-      </c>
-      <c r="E88" s="7" t="n">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="89" ht="14.3" customHeight="1">
-      <c r="A89" s="9" t="n"/>
-      <c r="B89" s="9" t="n"/>
-      <c r="C89" s="4" t="inlineStr">
-        <is>
-          <t>2.</t>
-        </is>
-      </c>
-      <c r="D89" s="7" t="inlineStr">
-        <is>
-          <t>pod.log-log</t>
-        </is>
-      </c>
-      <c r="E89" s="7" t="n">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="90" ht="14.3" customHeight="1">
-      <c r="A90" s="5" t="inlineStr">
-        <is>
-          <t>35.</t>
-        </is>
-      </c>
-      <c r="B90" s="5" t="inlineStr">
-        <is>
-          <t>pod.prz</t>
-        </is>
-      </c>
-      <c r="C90" s="5" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D90" s="6" t="inlineStr">
-        <is>
-          <t>pod.prz</t>
-        </is>
-      </c>
-      <c r="E90" s="6" t="n">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="91" ht="14.3" customHeight="1">
-      <c r="A91" s="4" t="inlineStr">
-        <is>
-          <t>36.</t>
-        </is>
-      </c>
-      <c r="B91" s="4" t="inlineStr">
-        <is>
-          <t>pod.stat</t>
-        </is>
-      </c>
-      <c r="C91" s="4" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D91" s="7" t="inlineStr">
-        <is>
-          <t>pod.stat-ra</t>
-        </is>
-      </c>
-      <c r="E91" s="7" t="n">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="92" ht="14.3" customHeight="1">
-      <c r="A92" s="5" t="inlineStr">
-        <is>
-          <t>37.</t>
-        </is>
-      </c>
-      <c r="B92" s="5" t="inlineStr">
-        <is>
-          <t>pod.żyw</t>
-        </is>
-      </c>
-      <c r="C92" s="5" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D92" s="6" t="inlineStr">
-        <is>
-          <t>pod.żyw</t>
-        </is>
-      </c>
-      <c r="E92" s="6" t="n">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="93" ht="14.3" customHeight="1">
-      <c r="A93" s="9" t="n"/>
-      <c r="B93" s="9" t="n"/>
-      <c r="C93" s="5" t="inlineStr">
-        <is>
-          <t>2.</t>
-        </is>
-      </c>
-      <c r="D93" s="6" t="inlineStr">
-        <is>
-          <t>pod.żyw-gas</t>
-        </is>
-      </c>
-      <c r="E93" s="6" t="n">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="94" ht="14.3" customHeight="1">
-      <c r="A94" s="4" t="inlineStr">
-        <is>
-          <t>38.</t>
-        </is>
-      </c>
-      <c r="B94" s="4" t="inlineStr">
-        <is>
-          <t>pr.est</t>
-        </is>
-      </c>
-      <c r="C94" s="4" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D94" s="7" t="inlineStr">
-        <is>
-          <t>pr.est-fry</t>
-        </is>
-      </c>
-      <c r="E94" s="7" t="n">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="95" ht="14.3" customHeight="1">
-      <c r="A95" s="5" t="inlineStr">
-        <is>
-          <t>39.</t>
-        </is>
-      </c>
-      <c r="B95" s="5" t="inlineStr">
-        <is>
-          <t>pr.fry</t>
-        </is>
-      </c>
-      <c r="C95" s="5" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D95" s="6" t="inlineStr">
-        <is>
-          <t>pr.fry-fry</t>
-        </is>
-      </c>
-      <c r="E95" s="6" t="n">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="96" ht="14.3" customHeight="1">
-      <c r="A96" s="8" t="n"/>
-      <c r="B96" s="8" t="n"/>
-      <c r="C96" s="5" t="inlineStr">
-        <is>
-          <t>2.</t>
-        </is>
-      </c>
-      <c r="D96" s="6" t="inlineStr">
-        <is>
-          <t>pr.fry-M-fry</t>
-        </is>
-      </c>
-      <c r="E96" s="6" t="n">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="97" ht="14.3" customHeight="1">
-      <c r="A97" s="8" t="n"/>
-      <c r="B97" s="8" t="n"/>
-      <c r="C97" s="5" t="inlineStr">
-        <is>
-          <t>3.</t>
-        </is>
-      </c>
-      <c r="D97" s="6" t="inlineStr">
-        <is>
-          <t>pr.fry.dam-fry</t>
-        </is>
-      </c>
-      <c r="E97" s="6" t="n">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="98" ht="14.3" customHeight="1">
-      <c r="A98" s="9" t="n"/>
-      <c r="B98" s="9" t="n"/>
-      <c r="C98" s="5" t="inlineStr">
-        <is>
-          <t>4.</t>
-        </is>
-      </c>
-      <c r="D98" s="6" t="inlineStr">
-        <is>
-          <t>pr.fry.men-fry</t>
-        </is>
-      </c>
-      <c r="E98" s="6" t="n">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="99" ht="14.3" customHeight="1">
-      <c r="A99" s="4" t="inlineStr">
-        <is>
-          <t>40.</t>
-        </is>
-      </c>
-      <c r="B99" s="4" t="inlineStr">
-        <is>
-          <t>pr.gas</t>
-        </is>
-      </c>
-      <c r="C99" s="4" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D99" s="7" t="inlineStr">
-        <is>
-          <t>pr.gas-gas</t>
-        </is>
-      </c>
-      <c r="E99" s="7" t="n">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="100" ht="14.3" customHeight="1">
-      <c r="A100" s="5" t="inlineStr">
-        <is>
-          <t>41.</t>
-        </is>
-      </c>
-      <c r="B100" s="5" t="inlineStr">
-        <is>
-          <t>pr.hot</t>
-        </is>
-      </c>
-      <c r="C100" s="5" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D100" s="6" t="inlineStr">
-        <is>
-          <t>pr.hot-hot</t>
-        </is>
-      </c>
-      <c r="E100" s="6" t="n">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="101" ht="14.3" customHeight="1">
-      <c r="A101" s="4" t="inlineStr">
-        <is>
-          <t>42.</t>
-        </is>
-      </c>
-      <c r="B101" s="4" t="inlineStr">
-        <is>
-          <t>pr.k.p.fry</t>
-        </is>
-      </c>
-      <c r="C101" s="4" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D101" s="7" t="inlineStr">
-        <is>
-          <t>pr.k.p.fry-fry</t>
-        </is>
-      </c>
-      <c r="E101" s="7" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="102" ht="14.3" customHeight="1">
-      <c r="A102" s="5" t="inlineStr">
-        <is>
-          <t>43.</t>
-        </is>
-      </c>
-      <c r="B102" s="5" t="inlineStr">
-        <is>
-          <t>pr.kosm</t>
-        </is>
-      </c>
-      <c r="C102" s="5" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D102" s="6" t="inlineStr">
-        <is>
-          <t>pr.kosm-fry</t>
-        </is>
-      </c>
-      <c r="E102" s="6" t="n">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="103" ht="14.3" customHeight="1">
-      <c r="A103" s="4" t="inlineStr">
-        <is>
-          <t>44.</t>
-        </is>
-      </c>
-      <c r="B103" s="4" t="inlineStr">
-        <is>
-          <t>pr.ob.inf</t>
-        </is>
-      </c>
-      <c r="C103" s="4" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D103" s="7" t="inlineStr">
-        <is>
-          <t>pr.ob.inf-gas</t>
-        </is>
-      </c>
-      <c r="E103" s="7" t="n">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="104" ht="14.3" customHeight="1">
-      <c r="A104" s="8" t="n"/>
-      <c r="B104" s="8" t="n"/>
-      <c r="C104" s="4" t="inlineStr">
-        <is>
-          <t>2.</t>
-        </is>
-      </c>
-      <c r="D104" s="7" t="inlineStr">
-        <is>
-          <t>pr.ob.inf-hot</t>
-        </is>
-      </c>
-      <c r="E104" s="7" t="n">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="105" ht="14.3" customHeight="1">
-      <c r="A105" s="8" t="n"/>
-      <c r="B105" s="8" t="n"/>
-      <c r="C105" s="4" t="inlineStr">
-        <is>
-          <t>3.</t>
-        </is>
-      </c>
-      <c r="D105" s="7" t="inlineStr">
-        <is>
-          <t>pr.ob.inf-j1</t>
-        </is>
-      </c>
-      <c r="E105" s="7" t="n">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="106" ht="14.3" customHeight="1">
-      <c r="A106" s="9" t="n"/>
-      <c r="B106" s="9" t="n"/>
-      <c r="C106" s="4" t="inlineStr">
-        <is>
-          <t>4.</t>
-        </is>
-      </c>
-      <c r="D106" s="7" t="inlineStr">
-        <is>
-          <t>pr.ob.inf-j2</t>
-        </is>
-      </c>
-      <c r="E106" s="7" t="n">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="107" ht="14.3" customHeight="1">
-      <c r="A107" s="5" t="inlineStr">
-        <is>
-          <t>45.</t>
-        </is>
-      </c>
-      <c r="B107" s="5" t="inlineStr">
-        <is>
-          <t>pr.ob.kon</t>
-        </is>
-      </c>
-      <c r="C107" s="5" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D107" s="6" t="inlineStr">
-        <is>
-          <t>pr.ob.kon-gas</t>
-        </is>
-      </c>
-      <c r="E107" s="6" t="n">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="108" ht="14.3" customHeight="1">
-      <c r="A108" s="9" t="n"/>
-      <c r="B108" s="9" t="n"/>
-      <c r="C108" s="5" t="inlineStr">
-        <is>
-          <t>2.</t>
-        </is>
-      </c>
-      <c r="D108" s="6" t="inlineStr">
-        <is>
-          <t>pr.ob.kon-hot</t>
-        </is>
-      </c>
-      <c r="E108" s="6" t="n">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="109" ht="14.3" customHeight="1">
-      <c r="A109" s="4" t="inlineStr">
-        <is>
-          <t>46.</t>
-        </is>
-      </c>
-      <c r="B109" s="4" t="inlineStr">
-        <is>
-          <t>pr.p.est</t>
-        </is>
-      </c>
-      <c r="C109" s="4" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D109" s="7" t="inlineStr">
-        <is>
-          <t>pr.p.est-fry</t>
-        </is>
-      </c>
-      <c r="E109" s="7" t="n">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="110" ht="14.3" customHeight="1">
-      <c r="A110" s="5" t="inlineStr">
-        <is>
-          <t>47.</t>
-        </is>
-      </c>
-      <c r="B110" s="5" t="inlineStr">
-        <is>
-          <t>prach</t>
-        </is>
-      </c>
-      <c r="C110" s="5" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D110" s="6" t="inlineStr">
-        <is>
-          <t>pr.rach-ra</t>
-        </is>
-      </c>
-      <c r="E110" s="6" t="n">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="111" ht="14.3" customHeight="1">
-      <c r="A111" s="4" t="inlineStr">
-        <is>
-          <t>48.</t>
-        </is>
-      </c>
-      <c r="B111" s="4" t="inlineStr">
-        <is>
-          <t>pr.s.k</t>
-        </is>
-      </c>
-      <c r="C111" s="4" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D111" s="7" t="inlineStr">
-        <is>
-          <t>pr.s.k-pła-ra</t>
-        </is>
-      </c>
-      <c r="E111" s="7" t="n">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="112" ht="14.3" customHeight="1">
-      <c r="A112" s="5" t="inlineStr">
-        <is>
-          <t>49.</t>
-        </is>
-      </c>
-      <c r="B112" s="5" t="inlineStr">
-        <is>
-          <t>pr.t.biu</t>
-        </is>
-      </c>
-      <c r="C112" s="5" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D112" s="6" t="inlineStr">
-        <is>
-          <t>pr.t.biu-ek</t>
-        </is>
-      </c>
-      <c r="E112" s="6" t="n">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="113" ht="14.3" customHeight="1">
-      <c r="A113" s="4" t="inlineStr">
-        <is>
-          <t>50.</t>
-        </is>
-      </c>
-      <c r="B113" s="4" t="inlineStr">
-        <is>
-          <t>pr.wyp.tech</t>
-        </is>
-      </c>
-      <c r="C113" s="4" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D113" s="7" t="inlineStr">
-        <is>
-          <t>pr.wyp.tech-gas</t>
-        </is>
-      </c>
-      <c r="E113" s="7" t="n">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="114" ht="14.3" customHeight="1">
-      <c r="A114" s="5" t="inlineStr">
-        <is>
-          <t>51.</t>
-        </is>
-      </c>
-      <c r="B114" s="5" t="inlineStr">
-        <is>
-          <t>pra.d.g</t>
-        </is>
-      </c>
-      <c r="C114" s="5" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D114" s="6" t="inlineStr">
-        <is>
-          <t>pra.d.g-ek</t>
-        </is>
-      </c>
-      <c r="E114" s="6" t="n">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="115" ht="14.3" customHeight="1">
-      <c r="A115" s="4" t="inlineStr">
-        <is>
-          <t>52.</t>
-        </is>
-      </c>
-      <c r="B115" s="4" t="inlineStr">
-        <is>
-          <t>pro.gos.fin</t>
-        </is>
-      </c>
-      <c r="C115" s="4" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D115" s="7" t="inlineStr">
-        <is>
-          <t>pro.gos.fin-ra</t>
-        </is>
-      </c>
-      <c r="E115" s="7" t="n">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="116" ht="14.3" customHeight="1">
-      <c r="A116" s="5" t="inlineStr">
-        <is>
-          <t>53.</t>
-        </is>
-      </c>
-      <c r="B116" s="5" t="inlineStr">
-        <is>
-          <t>przech.zap</t>
-        </is>
-      </c>
-      <c r="C116" s="5" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D116" s="6" t="inlineStr">
-        <is>
-          <t>przech.zap-log</t>
-        </is>
-      </c>
-      <c r="E116" s="6" t="n">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="117" ht="14.3" customHeight="1">
-      <c r="A117" s="4" t="inlineStr">
-        <is>
-          <t>54.</t>
-        </is>
-      </c>
-      <c r="B117" s="4" t="inlineStr">
-        <is>
-          <t>rach.fin</t>
-        </is>
-      </c>
-      <c r="C117" s="4" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D117" s="7" t="inlineStr">
-        <is>
-          <t>rach.fin-ra</t>
-        </is>
-      </c>
-      <c r="E117" s="7" t="n">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="118" ht="14.3" customHeight="1">
-      <c r="A118" s="5" t="inlineStr">
-        <is>
-          <t>55.</t>
-        </is>
-      </c>
-      <c r="B118" s="5" t="inlineStr">
-        <is>
-          <t>religia</t>
-        </is>
-      </c>
-      <c r="C118" s="5" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D118" s="6" t="inlineStr">
-        <is>
-          <t>religia</t>
-        </is>
-      </c>
-      <c r="E118" s="6" t="n">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="119" ht="14.3" customHeight="1">
-      <c r="A119" s="4" t="inlineStr">
-        <is>
-          <t>56.</t>
-        </is>
-      </c>
-      <c r="B119" s="4" t="inlineStr">
-        <is>
-          <t>stat</t>
-        </is>
-      </c>
-      <c r="C119" s="4" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D119" s="7" t="inlineStr">
-        <is>
-          <t>stat-ek</t>
-        </is>
-      </c>
-      <c r="E119" s="7" t="n">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="120" ht="14.3" customHeight="1">
-      <c r="A120" s="5" t="inlineStr">
-        <is>
-          <t>57.</t>
-        </is>
-      </c>
-      <c r="B120" s="5" t="inlineStr">
-        <is>
-          <t>t.fry</t>
-        </is>
-      </c>
-      <c r="C120" s="5" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D120" s="6" t="inlineStr">
-        <is>
-          <t>t.fry-fry</t>
-        </is>
-      </c>
-      <c r="E120" s="6" t="n">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="121" ht="14.3" customHeight="1">
-      <c r="A121" s="4" t="inlineStr">
-        <is>
-          <t>58.</t>
-        </is>
-      </c>
-      <c r="B121" s="4" t="inlineStr">
-        <is>
-          <t>us.w.gas</t>
-        </is>
-      </c>
-      <c r="C121" s="4" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D121" s="7" t="inlineStr">
-        <is>
-          <t>us.w.gas</t>
-        </is>
-      </c>
-      <c r="E121" s="7" t="n">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="122" ht="14.3" customHeight="1">
-      <c r="A122" s="9" t="n"/>
-      <c r="B122" s="9" t="n"/>
-      <c r="C122" s="4" t="inlineStr">
-        <is>
-          <t>2.</t>
-        </is>
-      </c>
-      <c r="D122" s="7" t="inlineStr">
-        <is>
-          <t>us.w.gas-gas</t>
-        </is>
-      </c>
-      <c r="E122" s="7" t="n">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="123" ht="14.3" customHeight="1">
-      <c r="A123" s="5" t="inlineStr">
-        <is>
-          <t>59.</t>
-        </is>
-      </c>
-      <c r="B123" s="5" t="inlineStr">
-        <is>
-          <t>w.f</t>
-        </is>
-      </c>
-      <c r="C123" s="5" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D123" s="6" t="inlineStr">
-        <is>
-          <t>w.f</t>
-        </is>
-      </c>
-      <c r="E123" s="6" t="n">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="124" ht="14.3" customHeight="1">
-      <c r="A124" s="8" t="n"/>
-      <c r="B124" s="8" t="n"/>
-      <c r="C124" s="5" t="inlineStr">
-        <is>
-          <t>2.</t>
-        </is>
-      </c>
-      <c r="D124" s="6" t="inlineStr">
-        <is>
-          <t>w.f-ek</t>
-        </is>
-      </c>
-      <c r="E124" s="6" t="n">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="125" ht="14.3" customHeight="1">
-      <c r="A125" s="8" t="n"/>
-      <c r="B125" s="8" t="n"/>
-      <c r="C125" s="5" t="inlineStr">
-        <is>
-          <t>3.</t>
-        </is>
-      </c>
-      <c r="D125" s="6" t="inlineStr">
-        <is>
-          <t>w.f-fry</t>
-        </is>
-      </c>
-      <c r="E125" s="6" t="n">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="126" ht="14.3" customHeight="1">
-      <c r="A126" s="8" t="n"/>
-      <c r="B126" s="8" t="n"/>
-      <c r="C126" s="5" t="inlineStr">
-        <is>
-          <t>4.</t>
-        </is>
-      </c>
-      <c r="D126" s="6" t="inlineStr">
-        <is>
-          <t>w.f-gas</t>
-        </is>
-      </c>
-      <c r="E126" s="6" t="n">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="127" ht="14.3" customHeight="1">
-      <c r="A127" s="8" t="n"/>
-      <c r="B127" s="8" t="n"/>
-      <c r="C127" s="5" t="inlineStr">
-        <is>
-          <t>5.</t>
-        </is>
-      </c>
-      <c r="D127" s="6" t="inlineStr">
-        <is>
-          <t>w.f-j1</t>
-        </is>
-      </c>
-      <c r="E127" s="6" t="n">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="128" ht="14.3" customHeight="1">
-      <c r="A128" s="8" t="n"/>
-      <c r="B128" s="8" t="n"/>
-      <c r="C128" s="5" t="inlineStr">
-        <is>
-          <t>6.</t>
-        </is>
-      </c>
-      <c r="D128" s="6" t="inlineStr">
-        <is>
-          <t>w.f-j2</t>
-        </is>
-      </c>
-      <c r="E128" s="6" t="n">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="129" ht="14.3" customHeight="1">
-      <c r="A129" s="8" t="n"/>
-      <c r="B129" s="8" t="n"/>
-      <c r="C129" s="5" t="inlineStr">
-        <is>
-          <t>7.</t>
-        </is>
-      </c>
-      <c r="D129" s="6" t="inlineStr">
-        <is>
-          <t>w.f-log</t>
-        </is>
-      </c>
-      <c r="E129" s="6" t="n">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="130" ht="14.3" customHeight="1">
-      <c r="A130" s="9" t="n"/>
-      <c r="B130" s="9" t="n"/>
-      <c r="C130" s="5" t="inlineStr">
-        <is>
-          <t>8.</t>
-        </is>
-      </c>
-      <c r="D130" s="6" t="inlineStr">
-        <is>
-          <t>w.f-ra</t>
-        </is>
-      </c>
-      <c r="E130" s="6" t="n">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="131" ht="14.3" customHeight="1">
-      <c r="A131" s="4" t="inlineStr">
-        <is>
-          <t>60.</t>
-        </is>
-      </c>
-      <c r="B131" s="4" t="inlineStr">
-        <is>
-          <t>w.o.s</t>
-        </is>
-      </c>
-      <c r="C131" s="4" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D131" s="7" t="inlineStr">
-        <is>
-          <t>w.o.s</t>
-        </is>
-      </c>
-      <c r="E131" s="7" t="n">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="132" ht="14.3" customHeight="1">
-      <c r="A132" s="5" t="inlineStr">
-        <is>
-          <t>61.</t>
-        </is>
-      </c>
-      <c r="B132" s="5" t="inlineStr">
-        <is>
-          <t>wło</t>
-        </is>
-      </c>
-      <c r="C132" s="5" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D132" s="6" t="inlineStr">
-        <is>
-          <t>wło</t>
-        </is>
-      </c>
-      <c r="E132" s="6" t="n">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="133" ht="14.3" customHeight="1">
-      <c r="A133" s="8" t="n"/>
-      <c r="B133" s="8" t="n"/>
-      <c r="C133" s="5" t="inlineStr">
-        <is>
-          <t>2.</t>
-        </is>
-      </c>
-      <c r="D133" s="6" t="inlineStr">
-        <is>
-          <t>wło-ek</t>
-        </is>
-      </c>
-      <c r="E133" s="6" t="n">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="134" ht="14.3" customHeight="1">
-      <c r="A134" s="8" t="n"/>
-      <c r="B134" s="8" t="n"/>
-      <c r="C134" s="5" t="inlineStr">
-        <is>
-          <t>3.</t>
-        </is>
-      </c>
-      <c r="D134" s="6" t="inlineStr">
-        <is>
-          <t>wło-fry</t>
-        </is>
-      </c>
-      <c r="E134" s="6" t="n">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="135" ht="14.3" customHeight="1">
-      <c r="A135" s="8" t="n"/>
-      <c r="B135" s="8" t="n"/>
-      <c r="C135" s="5" t="inlineStr">
-        <is>
-          <t>4.</t>
-        </is>
-      </c>
-      <c r="D135" s="6" t="inlineStr">
-        <is>
-          <t>wło-gas</t>
-        </is>
-      </c>
-      <c r="E135" s="6" t="n">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="136" ht="14.3" customHeight="1">
-      <c r="A136" s="8" t="n"/>
-      <c r="B136" s="8" t="n"/>
-      <c r="C136" s="5" t="inlineStr">
-        <is>
-          <t>5.</t>
-        </is>
-      </c>
-      <c r="D136" s="6" t="inlineStr">
-        <is>
-          <t>wło-hot</t>
-        </is>
-      </c>
-      <c r="E136" s="6" t="n">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="137" ht="14.3" customHeight="1">
-      <c r="A137" s="8" t="n"/>
-      <c r="B137" s="8" t="n"/>
-      <c r="C137" s="5" t="inlineStr">
-        <is>
-          <t>6.</t>
-        </is>
-      </c>
-      <c r="D137" s="6" t="inlineStr">
-        <is>
-          <t>wło-j1</t>
-        </is>
-      </c>
-      <c r="E137" s="6" t="n">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="138" ht="14.3" customHeight="1">
-      <c r="A138" s="8" t="n"/>
-      <c r="B138" s="8" t="n"/>
-      <c r="C138" s="5" t="inlineStr">
-        <is>
-          <t>7.</t>
-        </is>
-      </c>
-      <c r="D138" s="6" t="inlineStr">
-        <is>
-          <t>wło-j2</t>
-        </is>
-      </c>
-      <c r="E138" s="6" t="n">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="139" ht="14.3" customHeight="1">
-      <c r="A139" s="9" t="n"/>
-      <c r="B139" s="9" t="n"/>
-      <c r="C139" s="5" t="inlineStr">
-        <is>
-          <t>8.</t>
-        </is>
-      </c>
-      <c r="D139" s="6" t="inlineStr">
-        <is>
-          <t>wło-log</t>
-        </is>
-      </c>
-      <c r="E139" s="6" t="n">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="140" ht="14.3" customHeight="1">
-      <c r="A140" s="4" t="inlineStr">
-        <is>
-          <t>62.</t>
-        </is>
-      </c>
-      <c r="B140" s="4" t="inlineStr">
-        <is>
-          <t>z.wło</t>
-        </is>
-      </c>
-      <c r="C140" s="4" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D140" s="7" t="inlineStr">
-        <is>
-          <t>z.r.wło</t>
-        </is>
-      </c>
-      <c r="E140" s="7" t="n">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="141" ht="14.3" customHeight="1">
-      <c r="A141" s="5" t="inlineStr">
-        <is>
-          <t>63.</t>
-        </is>
-      </c>
-      <c r="B141" s="5" t="inlineStr">
-        <is>
-          <t>z.z.w</t>
-        </is>
-      </c>
-      <c r="C141" s="5" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D141" s="6" t="inlineStr">
-        <is>
-          <t>z.z.w</t>
-        </is>
-      </c>
-      <c r="E141" s="6" t="n">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="142" ht="14.3" customHeight="1">
-      <c r="A142" s="4" t="inlineStr">
-        <is>
-          <t>64.</t>
-        </is>
-      </c>
-      <c r="B142" s="4" t="inlineStr">
-        <is>
-          <t>zab.maj</t>
-        </is>
-      </c>
-      <c r="C142" s="4" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D142" s="7" t="inlineStr">
-        <is>
-          <t>zab.maj-log</t>
-        </is>
-      </c>
-      <c r="E142" s="7" t="n">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="143" ht="14.3" customHeight="1">
-      <c r="A143" s="5" t="inlineStr">
-        <is>
-          <t>65.</t>
-        </is>
-      </c>
-      <c r="B143" s="5" t="inlineStr">
-        <is>
-          <t>zaj.sport</t>
-        </is>
-      </c>
-      <c r="C143" s="5" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D143" s="6" t="inlineStr">
-        <is>
-          <t>zaj.sport</t>
-        </is>
-      </c>
-      <c r="E143" s="6" t="n">
-        <v>142</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="44">
-    <mergeCell ref="A67:A70"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="A88:A89"/>
-    <mergeCell ref="B22:B27"/>
-    <mergeCell ref="A123:A130"/>
-    <mergeCell ref="B86:B87"/>
-    <mergeCell ref="A72:A74"/>
-    <mergeCell ref="B77:B78"/>
-    <mergeCell ref="B121:B122"/>
-    <mergeCell ref="B123:B130"/>
-    <mergeCell ref="A103:A106"/>
-    <mergeCell ref="B82:B83"/>
-    <mergeCell ref="A132:A139"/>
-    <mergeCell ref="B67:B70"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="B64:B66"/>
-    <mergeCell ref="B88:B89"/>
-    <mergeCell ref="B2:B16"/>
-    <mergeCell ref="A86:A87"/>
-    <mergeCell ref="B58:B61"/>
-    <mergeCell ref="B107:B108"/>
-    <mergeCell ref="A64:A66"/>
-    <mergeCell ref="A95:A98"/>
-    <mergeCell ref="B103:B106"/>
-    <mergeCell ref="A35:A41"/>
-    <mergeCell ref="B35:B41"/>
-    <mergeCell ref="B132:B139"/>
-    <mergeCell ref="B45:B55"/>
-    <mergeCell ref="A2:A16"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="B72:B74"/>
-    <mergeCell ref="A77:A78"/>
-    <mergeCell ref="A121:A122"/>
-    <mergeCell ref="B95:B98"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="B92:B93"/>
-    <mergeCell ref="A22:A27"/>
-    <mergeCell ref="A92:A93"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="A107:A108"/>
-    <mergeCell ref="A82:A83"/>
-    <mergeCell ref="A45:A55"/>
-    <mergeCell ref="A58:A61"/>
+  <mergeCells count="12">
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A50:A53"/>
+    <mergeCell ref="B50:B53"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="B2:B8"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A30:A31"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>